<commit_message>
more app stuff. Need to fix empty summoner name
</commit_message>
<xml_diff>
--- a/v0/locations.xlsx
+++ b/v0/locations.xlsx
@@ -1,22 +1,23 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23929"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26626"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mmend\Desktop\RiotAPI\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/934d8c42a9f5e4dc/riot_api_git_clone_folder/Riot_Api/v0/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{54F16A60-C56D-49EE-B808-6D544082BE3D}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="1" documentId="13_ncr:1_{54F16A60-C56D-49EE-B808-6D544082BE3D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{31FEDC85-ED10-4AD3-91AC-F536EB00A581}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="3" xr2:uid="{2EF26C13-31AC-4153-8020-1A7F9321C13A}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="3" xr2:uid="{2EF26C13-31AC-4153-8020-1A7F9321C13A}"/>
   </bookViews>
   <sheets>
     <sheet name="Y dist" sheetId="2" r:id="rId1"/>
     <sheet name="normal dist" sheetId="1" r:id="rId2"/>
     <sheet name="working" sheetId="3" r:id="rId3"/>
-    <sheet name="Sheet1" sheetId="4" r:id="rId4"/>
+    <sheet name="Sheet2" sheetId="5" r:id="rId4"/>
+    <sheet name="Sheet1" sheetId="4" r:id="rId5"/>
   </sheets>
   <calcPr calcId="181029"/>
   <extLst>
@@ -28,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="131" uniqueCount="49">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="181" uniqueCount="59">
   <si>
     <t>championName</t>
   </si>
@@ -222,6 +223,36 @@
   </si>
   <si>
     <t>bot_area =[(16000,0), (6000,0), (6000,3500), (12000,4000), (13000,10000), (16000,10000)]</t>
+  </si>
+  <si>
+    <t>MatchId</t>
+  </si>
+  <si>
+    <t>ParticipantId</t>
+  </si>
+  <si>
+    <t>Role</t>
+  </si>
+  <si>
+    <t>ValidRoles</t>
+  </si>
+  <si>
+    <t>a</t>
+  </si>
+  <si>
+    <t>b</t>
+  </si>
+  <si>
+    <t>c</t>
+  </si>
+  <si>
+    <t>Jungle Flag</t>
+  </si>
+  <si>
+    <t>SupportFlag</t>
+  </si>
+  <si>
+    <t>posRole</t>
   </si>
 </sst>
 </file>
@@ -761,15 +792,15 @@
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
       <xdr:col>0</xdr:col>
-      <xdr:colOff>236220</xdr:colOff>
-      <xdr:row>0</xdr:row>
-      <xdr:rowOff>137160</xdr:rowOff>
+      <xdr:colOff>403860</xdr:colOff>
+      <xdr:row>1</xdr:row>
+      <xdr:rowOff>175260</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>5</xdr:col>
-      <xdr:colOff>213622</xdr:colOff>
-      <xdr:row>17</xdr:row>
-      <xdr:rowOff>145050</xdr:rowOff>
+      <xdr:colOff>381262</xdr:colOff>
+      <xdr:row>19</xdr:row>
+      <xdr:rowOff>270</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -792,7 +823,7 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="236220" y="137160"/>
+          <a:off x="403860" y="358140"/>
           <a:ext cx="3025402" cy="3116850"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
@@ -4379,7 +4410,7 @@
   <dimension ref="C8:AA29"/>
   <sheetViews>
     <sheetView topLeftCell="A5" zoomScale="81" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="W13" sqref="W13"/>
+      <selection activeCell="V21" sqref="V21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -4477,7 +4508,7 @@
         <v>41</v>
       </c>
       <c r="X11" t="str">
-        <f t="shared" ref="X11:X14" si="1">X10&amp;W11&amp;", "</f>
+        <f t="shared" ref="X11:X13" si="1">X10&amp;W11&amp;", "</f>
         <v xml:space="preserve">[(0,16000), (0,6000), (3950,6000), </v>
       </c>
       <c r="Z11" s="5" t="s">
@@ -5011,11 +5042,406 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{93D0E6AF-9E66-4E4F-B2AE-8D07D80CFD00}">
+  <dimension ref="G5:Q26"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="Q19" sqref="Q19"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="8" max="8" width="11.33203125" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="11.33203125" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="9.6640625" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="10.5546875" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="5" spans="7:17" x14ac:dyDescent="0.3">
+      <c r="G5" t="s">
+        <v>49</v>
+      </c>
+      <c r="H5" t="s">
+        <v>50</v>
+      </c>
+      <c r="I5" t="s">
+        <v>51</v>
+      </c>
+      <c r="J5" t="s">
+        <v>52</v>
+      </c>
+      <c r="M5" t="s">
+        <v>49</v>
+      </c>
+      <c r="N5" t="s">
+        <v>50</v>
+      </c>
+      <c r="O5" t="s">
+        <v>56</v>
+      </c>
+      <c r="P5" t="s">
+        <v>57</v>
+      </c>
+      <c r="Q5" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="6" spans="7:17" x14ac:dyDescent="0.3">
+      <c r="G6" t="s">
+        <v>53</v>
+      </c>
+      <c r="H6">
+        <v>1</v>
+      </c>
+      <c r="M6" t="s">
+        <v>53</v>
+      </c>
+      <c r="N6">
+        <v>1</v>
+      </c>
+      <c r="O6" t="b">
+        <v>1</v>
+      </c>
+      <c r="P6" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="7" spans="7:17" x14ac:dyDescent="0.3">
+      <c r="G7" t="s">
+        <v>53</v>
+      </c>
+      <c r="H7">
+        <v>2</v>
+      </c>
+      <c r="M7" t="s">
+        <v>53</v>
+      </c>
+      <c r="N7">
+        <v>2</v>
+      </c>
+      <c r="O7" t="b">
+        <v>0</v>
+      </c>
+      <c r="P7" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="8" spans="7:17" x14ac:dyDescent="0.3">
+      <c r="G8" t="s">
+        <v>53</v>
+      </c>
+      <c r="H8">
+        <v>3</v>
+      </c>
+      <c r="M8" t="s">
+        <v>53</v>
+      </c>
+      <c r="N8">
+        <v>3</v>
+      </c>
+      <c r="O8" t="b">
+        <v>0</v>
+      </c>
+      <c r="P8" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="9" spans="7:17" x14ac:dyDescent="0.3">
+      <c r="G9" t="s">
+        <v>53</v>
+      </c>
+      <c r="H9">
+        <v>4</v>
+      </c>
+      <c r="M9" t="s">
+        <v>53</v>
+      </c>
+      <c r="N9">
+        <v>4</v>
+      </c>
+      <c r="O9" t="b">
+        <v>0</v>
+      </c>
+      <c r="P9" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="10" spans="7:17" x14ac:dyDescent="0.3">
+      <c r="G10" t="s">
+        <v>53</v>
+      </c>
+      <c r="H10">
+        <v>5</v>
+      </c>
+      <c r="M10" t="s">
+        <v>53</v>
+      </c>
+      <c r="N10">
+        <v>5</v>
+      </c>
+      <c r="O10" t="b">
+        <v>0</v>
+      </c>
+      <c r="P10" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="11" spans="7:17" x14ac:dyDescent="0.3">
+      <c r="G11" t="s">
+        <v>53</v>
+      </c>
+      <c r="H11">
+        <v>6</v>
+      </c>
+      <c r="M11" t="s">
+        <v>53</v>
+      </c>
+      <c r="N11">
+        <v>6</v>
+      </c>
+      <c r="O11" t="b">
+        <v>0</v>
+      </c>
+      <c r="P11" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="12" spans="7:17" x14ac:dyDescent="0.3">
+      <c r="G12" t="s">
+        <v>53</v>
+      </c>
+      <c r="H12">
+        <v>7</v>
+      </c>
+      <c r="M12" t="s">
+        <v>53</v>
+      </c>
+      <c r="N12">
+        <v>7</v>
+      </c>
+      <c r="O12" t="b">
+        <v>0</v>
+      </c>
+      <c r="P12" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="13" spans="7:17" x14ac:dyDescent="0.3">
+      <c r="G13" t="s">
+        <v>53</v>
+      </c>
+      <c r="H13">
+        <v>8</v>
+      </c>
+      <c r="M13" t="s">
+        <v>53</v>
+      </c>
+      <c r="N13">
+        <v>8</v>
+      </c>
+      <c r="O13" t="b">
+        <v>0</v>
+      </c>
+      <c r="P13" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="14" spans="7:17" x14ac:dyDescent="0.3">
+      <c r="G14" t="s">
+        <v>53</v>
+      </c>
+      <c r="H14">
+        <v>9</v>
+      </c>
+      <c r="M14" t="s">
+        <v>53</v>
+      </c>
+      <c r="N14">
+        <v>9</v>
+      </c>
+      <c r="O14" t="b">
+        <v>0</v>
+      </c>
+      <c r="P14" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="15" spans="7:17" x14ac:dyDescent="0.3">
+      <c r="G15" t="s">
+        <v>53</v>
+      </c>
+      <c r="H15">
+        <v>10</v>
+      </c>
+      <c r="M15" t="s">
+        <v>53</v>
+      </c>
+      <c r="N15">
+        <v>10</v>
+      </c>
+      <c r="O15" t="b">
+        <v>1</v>
+      </c>
+      <c r="P15" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="16" spans="7:17" x14ac:dyDescent="0.3">
+      <c r="G16" t="s">
+        <v>54</v>
+      </c>
+      <c r="H16">
+        <v>1</v>
+      </c>
+      <c r="M16" t="s">
+        <v>54</v>
+      </c>
+      <c r="N16">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="17" spans="7:14" x14ac:dyDescent="0.3">
+      <c r="G17" t="s">
+        <v>54</v>
+      </c>
+      <c r="H17">
+        <v>2</v>
+      </c>
+      <c r="M17" t="s">
+        <v>54</v>
+      </c>
+      <c r="N17">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="18" spans="7:14" x14ac:dyDescent="0.3">
+      <c r="G18" t="s">
+        <v>54</v>
+      </c>
+      <c r="H18">
+        <v>3</v>
+      </c>
+      <c r="M18" t="s">
+        <v>54</v>
+      </c>
+      <c r="N18">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="19" spans="7:14" x14ac:dyDescent="0.3">
+      <c r="G19" t="s">
+        <v>54</v>
+      </c>
+      <c r="H19">
+        <v>4</v>
+      </c>
+      <c r="M19" t="s">
+        <v>54</v>
+      </c>
+      <c r="N19">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="20" spans="7:14" x14ac:dyDescent="0.3">
+      <c r="G20" t="s">
+        <v>54</v>
+      </c>
+      <c r="H20">
+        <v>5</v>
+      </c>
+      <c r="M20" t="s">
+        <v>54</v>
+      </c>
+      <c r="N20">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="21" spans="7:14" x14ac:dyDescent="0.3">
+      <c r="G21" t="s">
+        <v>54</v>
+      </c>
+      <c r="H21">
+        <v>6</v>
+      </c>
+      <c r="M21" t="s">
+        <v>54</v>
+      </c>
+      <c r="N21">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="22" spans="7:14" x14ac:dyDescent="0.3">
+      <c r="G22" t="s">
+        <v>54</v>
+      </c>
+      <c r="H22">
+        <v>7</v>
+      </c>
+      <c r="M22" t="s">
+        <v>54</v>
+      </c>
+      <c r="N22">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="23" spans="7:14" x14ac:dyDescent="0.3">
+      <c r="G23" t="s">
+        <v>54</v>
+      </c>
+      <c r="H23">
+        <v>8</v>
+      </c>
+      <c r="M23" t="s">
+        <v>54</v>
+      </c>
+      <c r="N23">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="24" spans="7:14" x14ac:dyDescent="0.3">
+      <c r="G24" t="s">
+        <v>54</v>
+      </c>
+      <c r="H24">
+        <v>9</v>
+      </c>
+      <c r="M24" t="s">
+        <v>54</v>
+      </c>
+      <c r="N24">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="25" spans="7:14" x14ac:dyDescent="0.3">
+      <c r="G25" t="s">
+        <v>54</v>
+      </c>
+      <c r="H25">
+        <v>10</v>
+      </c>
+      <c r="M25" t="s">
+        <v>54</v>
+      </c>
+      <c r="N25">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="26" spans="7:14" x14ac:dyDescent="0.3">
+      <c r="G26" t="s">
+        <v>55</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{903D0598-6620-4F82-BCF2-7A8E8A1EC120}">
   <dimension ref="H6:H12"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A2" workbookViewId="0">
-      <selection activeCell="H13" sqref="H13"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="L21" sqref="L21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>

</xml_diff>